<commit_message>
checking in and saying Hi.
</commit_message>
<xml_diff>
--- a/FinalSchedule.xlsx
+++ b/FinalSchedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Monday</t>
   </si>
@@ -78,16 +78,26 @@
     <t>FP: Ch 12 (J)
 FP: Intro (J &amp; B)
 FP: Appendices (B)</t>
+  </si>
+  <si>
+    <t>FP = First Pass
+AR = Author Review</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -175,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -215,6 +225,12 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -547,10 +563,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B2:H32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -811,8 +830,10 @@
         <v>6</v>
       </c>
       <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
+      <c r="E16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="15"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
     </row>
@@ -878,11 +899,15 @@
       <c r="B32" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E16:F16"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="98" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>